<commit_message>
added 'Belgium' to ERMG revenue survey output
</commit_message>
<xml_diff>
--- a/data/interim/economical/ERMG_revenue_survey.xlsx
+++ b/data/interim/economical/ERMG_revenue_survey.xlsx
@@ -3018,37 +3018,37 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0</v>
+        <v>-32.81588623434916</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>-36.24548956597219</v>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>-32.6366242868741</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>-33.53330230258769</v>
       </c>
       <c r="F65" t="n">
-        <v>0</v>
+        <v>-31.79406828509521</v>
       </c>
       <c r="G65" t="n">
-        <v>0</v>
+        <v>-28.88833918996838</v>
       </c>
       <c r="H65" t="n">
-        <v>0</v>
+        <v>-30.59865647806746</v>
       </c>
       <c r="I65" t="n">
-        <v>0</v>
+        <v>-25.77335156301567</v>
       </c>
       <c r="J65" t="n">
-        <v>0</v>
+        <v>-23.29390289135626</v>
       </c>
       <c r="K65" t="n">
-        <v>0</v>
+        <v>-17.33111597263522</v>
       </c>
       <c r="L65" t="n">
-        <v>0</v>
+        <v>-12.56852078018352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>